<commit_message>
Revision for first Public release
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -32,6 +32,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Nombre: si tiene dos, solo el primero, por ejemplo:
 Ana maría = Ana</t>
@@ -45,6 +46,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Apellidos</t>
         </r>
@@ -57,6 +59,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Nombre de usuario:
 1 – No puede tener espacios, tildes, ~n, ü..
@@ -68,6 +71,7 @@
             <color rgb="FF0000FF"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">pepe@a.cu</t>
         </r>
@@ -76,6 +80,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">)
 3 – Todo en minusculas
@@ -91,6 +96,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Grupo, que será la unidad organizativa a la que pertenece primariamente
 O sea este puede ser de un subgrupo de la dirección, pero en esencia es dirección
@@ -107,6 +113,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Grupo de permisos para el proxy, son grupos en el AD 
 </t>
@@ -117,6 +124,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Vip</t>
         </r>
@@ -125,6 +133,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">: Acceso a todo a todas horas
 </t>
@@ -135,6 +144,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Normal</t>
         </r>
@@ -143,6 +153,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">: Acceso a lo normalmente permitido en horario laboral
 </t>
@@ -153,6 +164,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Nacional</t>
         </r>
@@ -161,6 +173,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">: Solo a *.cu en horario laboral
 </t>
@@ -171,6 +184,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Local</t>
         </r>
@@ -179,6 +193,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">: Solo a los recursos de la red, no tiene acceso a internet ni a la nacional
 </t>
@@ -192,6 +207,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Accesos del correo son grupos en el AD
 - Internacional
@@ -771,6 +787,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -792,12 +809,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -941,15 +960,17 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,7 +2116,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>